<commit_message>
lx: more qp funcs & estu
</commit_message>
<xml_diff>
--- a/Dictionary.xlsx
+++ b/Dictionary.xlsx
@@ -23544,13 +23544,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23563,7 +23563,7 @@
     <col min="6" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>7446</v>
       </c>
@@ -23580,148 +23580,154 @@
         <v>7385</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>7386</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>7450</v>
+        <v>7403</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>1117</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>7474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A3" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>7451</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>7387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7404</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>7473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>7388</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>7452</v>
+        <v>7411</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>1126</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>7474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>7453</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>7389</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="27" hidden="1" x14ac:dyDescent="0.15">
+        <v>7412</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>7474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>7390</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>7454</v>
+        <v>7414</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A7" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>7455</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>7391</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="27" hidden="1" x14ac:dyDescent="0.15">
+        <v>7418</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>7469</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>7474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>7449</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>7392</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>7456</v>
+      <c r="C8" s="35" t="s">
+        <v>7419</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>1093</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>7473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="31">
-        <v>1</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>7449</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>7457</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>7393</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>7470</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>7471</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>7473</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A10" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>7394</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>7458</v>
+        <v>7421</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7472</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>7473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="31">
         <v>1</v>
       </c>
@@ -23729,13 +23735,16 @@
         <v>7449</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>7459</v>
+        <v>7386</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>7395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7450</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="31">
         <v>1</v>
       </c>
@@ -23743,16 +23752,13 @@
         <v>7449</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>7396</v>
+        <v>7451</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>7460</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7387</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="31">
         <v>1</v>
       </c>
@@ -23760,13 +23766,16 @@
         <v>7449</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>7461</v>
+        <v>7388</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>7397</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7452</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -23774,16 +23783,13 @@
         <v>7449</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>7398</v>
+        <v>7453</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>7462</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" s="31">
         <v>1</v>
       </c>
@@ -23791,13 +23797,16 @@
         <v>7449</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>7463</v>
+        <v>7390</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>7399</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7454</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="31">
         <v>1</v>
       </c>
@@ -23805,33 +23814,30 @@
         <v>7449</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>7400</v>
+        <v>7455</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>7464</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7391</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="31">
         <v>1</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>7465</v>
+        <v>7449</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>31</v>
+        <v>7392</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>1052</v>
+        <v>7456</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="31">
         <v>1</v>
       </c>
@@ -23839,10 +23845,13 @@
         <v>7449</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>7401</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7457</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>7393</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="31">
         <v>1</v>
       </c>
@@ -23850,10 +23859,16 @@
         <v>7449</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>7402</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7394</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>7458</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="31">
         <v>1</v>
       </c>
@@ -23861,64 +23876,61 @@
         <v>7449</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>7466</v>
+        <v>7459</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>7467</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>7403</v>
+        <v>7396</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>7460</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>7474</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>7404</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>1146</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>7473</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7461</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>7397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="31">
         <v>1</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>7465</v>
+        <v>7449</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>33</v>
+        <v>7398</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>7405</v>
+        <v>7462</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="31">
         <v>1</v>
       </c>
@@ -23926,10 +23938,13 @@
         <v>7449</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>7406</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7463</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>7399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="31">
         <v>1</v>
       </c>
@@ -23937,21 +23952,33 @@
         <v>7449</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>7407</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7400</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>7464</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="31">
         <v>1</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>7449</v>
+        <v>7465</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>7408</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="31">
         <v>1</v>
       </c>
@@ -23959,10 +23986,10 @@
         <v>7449</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>7409</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7401</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="31">
         <v>1</v>
       </c>
@@ -23970,47 +23997,41 @@
         <v>7449</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>7410</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="27" hidden="1" x14ac:dyDescent="0.15">
+        <v>7402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>7411</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>1126</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>7474</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7466</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>7467</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>7449</v>
+        <v>7465</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>7412</v>
+        <v>33</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>7405</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>1128</v>
-      </c>
-      <c r="F30" s="33" t="s">
-        <v>7474</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="31">
         <v>1</v>
       </c>
@@ -24018,27 +24039,21 @@
         <v>7449</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>7413</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7406</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>7414</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
+        <v>7407</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="31">
         <v>1</v>
       </c>
@@ -24046,13 +24061,10 @@
         <v>7449</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>7415</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>7468</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7408</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="31">
         <v>1</v>
       </c>
@@ -24060,13 +24072,10 @@
         <v>7449</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>7416</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>7409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="31">
         <v>1</v>
       </c>
@@ -24074,95 +24083,86 @@
         <v>7449</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>7417</v>
+        <v>7410</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="67.5" hidden="1" x14ac:dyDescent="0.15">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>7449</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>7418</v>
+        <v>7413</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>7469</v>
-      </c>
-      <c r="F36" s="33" t="s">
-        <v>7474</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A37" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>7449</v>
       </c>
-      <c r="C37" s="35" t="s">
-        <v>7419</v>
+      <c r="C37" s="31" t="s">
+        <v>7415</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F37" s="33" t="s">
-        <v>7473</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+        <v>7468</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="31">
-        <v>0</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>7470</v>
+        <v>1</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>7449</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>7416</v>
       </c>
       <c r="E38" s="32" t="s">
-        <v>7471</v>
-      </c>
-      <c r="F38" s="33" t="s">
-        <v>7473</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="31">
         <v>1</v>
       </c>
       <c r="B39" s="31" t="s">
+        <v>7449</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>7417</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="31">
+        <v>1</v>
+      </c>
+      <c r="B40" s="31" t="s">
         <v>7465</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C40" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D40" s="31" t="s">
         <v>1046</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="E40" s="32" t="s">
         <v>7420</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="31">
-        <v>0</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>7449</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>7421</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>7472</v>
-      </c>
-      <c r="F40" s="33" t="s">
-        <v>7473</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="31">
         <v>1</v>
       </c>
@@ -24179,7 +24179,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="31">
         <v>1</v>
       </c>
@@ -24193,7 +24193,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="31">
         <v>1</v>
       </c>
@@ -24204,7 +24204,7 @@
         <v>7424</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="31">
         <v>1</v>
       </c>
@@ -24215,7 +24215,7 @@
         <v>7425</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="31">
         <v>1</v>
       </c>
@@ -24226,7 +24226,7 @@
         <v>7426</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="31">
         <v>1</v>
       </c>
@@ -24237,7 +24237,7 @@
         <v>7427</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="31">
         <v>1</v>
       </c>
@@ -24248,7 +24248,7 @@
         <v>7428</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="31">
         <v>1</v>
       </c>
@@ -24259,7 +24259,7 @@
         <v>7429</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="31">
         <v>1</v>
       </c>
@@ -24270,7 +24270,7 @@
         <v>7430</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="31">
         <v>1</v>
       </c>
@@ -24287,7 +24287,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="31">
         <v>2</v>
       </c>
@@ -24298,7 +24298,7 @@
         <v>7431</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="31">
         <v>2</v>
       </c>
@@ -24315,7 +24315,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="31">
         <v>2</v>
       </c>
@@ -24332,7 +24332,7 @@
         <v>7433</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="31">
         <v>2</v>
       </c>
@@ -24349,7 +24349,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="31">
         <v>2</v>
       </c>
@@ -24366,7 +24366,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="31">
         <v>2</v>
       </c>
@@ -24383,7 +24383,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="31">
         <v>2</v>
       </c>
@@ -24397,7 +24397,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="31">
         <v>2</v>
       </c>
@@ -24411,7 +24411,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A59" s="31">
         <v>2</v>
       </c>
@@ -24428,7 +24428,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="31">
         <v>2</v>
       </c>
@@ -24442,7 +24442,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="31">
         <v>2</v>
       </c>
@@ -24456,7 +24456,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="31">
         <v>2</v>
       </c>
@@ -24473,7 +24473,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="31">
         <v>2</v>
       </c>
@@ -24490,7 +24490,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="31">
         <v>2</v>
       </c>
@@ -24507,7 +24507,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="31">
         <v>2</v>
       </c>
@@ -24524,7 +24524,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="31">
         <v>2</v>
       </c>
@@ -24541,7 +24541,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="31">
         <v>2</v>
       </c>
@@ -24558,7 +24558,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="31">
         <v>2</v>
       </c>
@@ -24575,7 +24575,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="31">
         <v>2</v>
       </c>
@@ -24592,7 +24592,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="31">
         <v>2</v>
       </c>
@@ -24609,7 +24609,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="31">
         <v>2</v>
       </c>
@@ -24626,7 +24626,7 @@
         <v>7441</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="31">
         <v>2</v>
       </c>
@@ -24643,7 +24643,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="31">
         <v>2</v>
       </c>
@@ -24660,7 +24660,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="31">
         <v>2</v>
       </c>
@@ -24677,7 +24677,7 @@
         <v>7442</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="31">
         <v>2</v>
       </c>
@@ -24694,7 +24694,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A76" s="31">
         <v>2</v>
       </c>
@@ -24711,7 +24711,7 @@
         <v>7443</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="31">
         <v>2</v>
       </c>
@@ -24728,7 +24728,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="31">
         <v>2</v>
       </c>
@@ -24739,7 +24739,7 @@
         <v>7444</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="31">
         <v>2</v>
       </c>
@@ -24750,7 +24750,7 @@
         <v>7445</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="31">
         <v>2</v>
       </c>
@@ -24767,7 +24767,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="31">
         <v>2</v>
       </c>
@@ -24784,7 +24784,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="31">
         <v>2</v>
       </c>
@@ -24815,11 +24815,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F82">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="lx"/>
-      </filters>
-    </filterColumn>
+    <sortState ref="A2:F82">
+      <sortCondition ref="A1:A82"/>
+    </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">

</xml_diff>